<commit_message>
Updated Financial Snapshot and Modules
</commit_message>
<xml_diff>
--- a/public/Ratios.xlsx
+++ b/public/Ratios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anakha Ajkumar\Downloads\dashboards\dashboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEEbugg\Desktop\AJA\2023\Vittora-AFA\WebApp\VittoraDashboards_A\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F31F44-06DF-43D6-ABA2-377C4FA59CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7035"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,7 +239,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,22 +519,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A12" sqref="A12:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -561,7 +562,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -575,7 +576,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -589,7 +590,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -603,7 +604,7 @@
         <v>116.43</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -617,7 +618,7 @@
         <v>171.59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -631,7 +632,7 @@
         <v>0.1017</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -645,21 +646,21 @@
         <v>0.76459999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1">
-        <v>0.1658</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -673,21 +674,21 @@
         <v>0.18820000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1">
-        <v>0.23699999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.1658</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -701,7 +702,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -715,7 +716,7 @@
         <v>5.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -729,7 +730,7 @@
         <v>4.0599999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -743,7 +744,7 @@
         <v>3.9399999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -757,7 +758,7 @@
         <v>12.34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -771,7 +772,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -785,7 +786,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -799,7 +800,7 @@
         <v>5.14507772020725</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>

</xml_diff>